<commit_message>
4.2 per facade calculated in Power_AC_Sum dataframe
</commit_message>
<xml_diff>
--- a/annualyieldpermodule.xlsx
+++ b/annualyieldpermodule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fb00dc8ed84c692/Documents/Utrecht University/Energy in Built/6.2 Photovoltaic (PV) systems^J irradiance and PV performance evaluation/utrechtsmartdistricpartA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="47" documentId="8_{EC9B7BA5-3176-4077-AEDA-D8135839D5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EB71CABC-B001-419B-8B40-18D13446C5E8}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{EC9B7BA5-3176-4077-AEDA-D8135839D5B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{875E6B3D-D646-45CA-930B-B239222DB6C3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{AD5D5653-035F-443A-A3B2-9117DE18EA5C}"/>
   </bookViews>
@@ -474,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7560010-2E6C-46A7-B5A5-A2D6BE8F529C}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -485,7 +485,7 @@
     <col min="5" max="5" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -502,7 +502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>14</v>
       </c>
@@ -519,12 +519,8 @@
         <f>C2/D2</f>
         <v>165.69022777777778</v>
       </c>
-      <c r="G2" s="4">
-        <f>E2-E4</f>
-        <v>39.801368710420263</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
@@ -542,7 +538,7 @@
         <v>86.841113888888884</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>14</v>
       </c>
@@ -560,7 +556,7 @@
         <v>125.88885906735752</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>15</v>
       </c>
@@ -577,12 +573,8 @@
         <f t="shared" si="0"/>
         <v>116.13786666666665</v>
       </c>
-      <c r="G5" s="4">
-        <f t="shared" ref="G5" si="1">E5-E7</f>
-        <v>27.330183246977526</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>15</v>
       </c>
@@ -600,7 +592,7 @@
         <v>61.123337500000005</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>15</v>
       </c>
@@ -618,7 +610,7 @@
         <v>88.807683419689127</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>16</v>
       </c>
@@ -635,12 +627,8 @@
         <f t="shared" si="0"/>
         <v>143.5893468253968</v>
       </c>
-      <c r="G8" s="4">
-        <f t="shared" ref="G8" si="2">E8-E10</f>
-        <v>34.599469623324268</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -658,7 +646,7 @@
         <v>74.977368055555559</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>16</v>
       </c>
@@ -676,7 +664,7 @@
         <v>108.98987720207253</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>17</v>
       </c>
@@ -693,12 +681,8 @@
         <f t="shared" si="0"/>
         <v>147.76748809523809</v>
       </c>
-      <c r="G11" s="4">
-        <f t="shared" ref="G11" si="3">E11-E13</f>
-        <v>35.216654934616329</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -716,7 +700,7 @@
         <v>77.364945833333337</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
@@ -734,7 +718,7 @@
         <v>112.55083316062176</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -751,12 +735,8 @@
         <f t="shared" si="0"/>
         <v>93.477615873015878</v>
       </c>
-      <c r="G14" s="4">
-        <f t="shared" ref="G14" si="4">E14-E16</f>
-        <v>21.844208619129859</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>18</v>
       </c>
@@ -774,7 +754,7 @@
         <v>49.338095833333334</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>18</v>
       </c>
@@ -792,7 +772,7 @@
         <v>71.63340725388602</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
@@ -809,12 +789,8 @@
         <f t="shared" si="0"/>
         <v>209.03917063492065</v>
       </c>
-      <c r="G17" s="4">
-        <f t="shared" ref="G17" si="5">E17-E19</f>
-        <v>50.436043173780746</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>6</v>
       </c>
@@ -832,7 +808,7 @@
         <v>109.68727916666667</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>6</v>
       </c>
@@ -850,7 +826,7 @@
         <v>158.60312746113991</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -867,12 +843,8 @@
         <f t="shared" si="0"/>
         <v>129.90182619047619</v>
       </c>
-      <c r="G20" s="4">
-        <f t="shared" ref="G20" si="6">E20-E22</f>
-        <v>30.882881112755982</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
@@ -890,7 +862,7 @@
         <v>67.659280555555569</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>7</v>
       </c>
@@ -908,7 +880,7 @@
         <v>99.018945077720204</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -925,12 +897,8 @@
         <f t="shared" si="0"/>
         <v>145.17481507936506</v>
       </c>
-      <c r="G23" s="4">
-        <f t="shared" ref="G23" si="7">E23-E25</f>
-        <v>34.302852903199252</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -948,7 +916,7 @@
         <v>76.420483333333337</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
         <v>8</v>
       </c>
@@ -966,7 +934,7 @@
         <v>110.87196217616581</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -983,12 +951,8 @@
         <f t="shared" si="0"/>
         <v>199.68055634920634</v>
       </c>
-      <c r="G26" s="4">
-        <f t="shared" ref="G26" si="8">E26-E28</f>
-        <v>48.51258018340323</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>9</v>
       </c>
@@ -1006,7 +970,7 @@
         <v>104.36345833333333</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>9</v>
       </c>
@@ -1024,7 +988,7 @@
         <v>151.16797616580311</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -1041,12 +1005,8 @@
         <f t="shared" si="0"/>
         <v>219.99817936507935</v>
       </c>
-      <c r="G29" s="4">
-        <f t="shared" ref="G29" si="9">E29-E31</f>
-        <v>53.407848795131144</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
         <v>10</v>
       </c>
@@ -1064,7 +1024,7 @@
         <v>115.33236111111111</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1082,7 +1042,7 @@
         <v>166.59033056994821</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
         <v>11</v>
       </c>
@@ -1098,10 +1058,6 @@
       <c r="E32" s="4">
         <f t="shared" si="0"/>
         <v>210.72316507936509</v>
-      </c>
-      <c r="G32" s="4">
-        <f t="shared" ref="G32" si="10">E32-E34</f>
-        <v>50.848098239986854</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>